<commit_message>
added feat for borough
</commit_message>
<xml_diff>
--- a/cut_income-of-tax-payers.xlsx
+++ b/cut_income-of-tax-payers.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve">Area</t>
   </si>
@@ -39,6 +39,18 @@
   </si>
   <si>
     <t xml:space="preserve">Median £</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crime rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fare Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population * 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop density 10000/km^2</t>
   </si>
   <si>
     <t xml:space="preserve">City of London</t>
@@ -144,13 +156,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="#,##0_);\(#,##0\)"/>
     <numFmt numFmtId="167" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -201,6 +214,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -232,7 +251,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="30">
+  <cellStyleXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -284,16 +303,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -302,15 +329,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="29" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="31" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -318,8 +349,16 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="18">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
@@ -334,8 +373,10 @@
     <cellStyle name="Normal 2 2" xfId="25"/>
     <cellStyle name="Normal 3" xfId="26"/>
     <cellStyle name="Normal 4" xfId="27"/>
-    <cellStyle name="Normal_01IRS0314" xfId="28"/>
-    <cellStyle name="Row_Headings" xfId="29"/>
+    <cellStyle name="Normal 6" xfId="28"/>
+    <cellStyle name="Normal_01IRS0314" xfId="29"/>
+    <cellStyle name="Normal_Sheet3" xfId="30"/>
+    <cellStyle name="Row_Headings" xfId="31"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -345,26 +386,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="972" min="7" style="1" width="10.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="973" style="0" width="14.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="971" min="9" style="1" width="10.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="972" style="0" width="14.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -380,12 +423,24 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5" t="n">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6" t="n">
         <v>11000</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -394,12 +449,24 @@
       <c r="D2" s="1" t="n">
         <v>60000</v>
       </c>
+      <c r="E2" s="1" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>8.71</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>3.241</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5" t="n">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>85000</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -408,12 +475,24 @@
       <c r="D3" s="1" t="n">
         <v>23900</v>
       </c>
+      <c r="E3" s="7" t="n">
+        <v>70.8999321902548</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="H3" s="8" t="n">
+        <v>5871</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5" t="n">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>188000</v>
       </c>
       <c r="C4" s="1" t="n">
@@ -422,12 +501,24 @@
       <c r="D4" s="1" t="n">
         <v>28700</v>
       </c>
+      <c r="E4" s="7" t="n">
+        <v>55.8144233234823</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>392.14</v>
+      </c>
+      <c r="H4" s="8" t="n">
+        <v>4520</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5" t="n">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>122000</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -436,12 +527,24 @@
       <c r="D5" s="1" t="n">
         <v>26900</v>
       </c>
+      <c r="E5" s="7" t="n">
+        <v>45.6079424742605</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>247.36</v>
+      </c>
+      <c r="H5" s="8" t="n">
+        <v>4100</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="5" t="n">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="n">
         <v>155000</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -450,12 +553,24 @@
       <c r="D6" s="1" t="n">
         <v>24700</v>
       </c>
+      <c r="E6" s="7" t="n">
+        <v>70.789693347225</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>330.8</v>
+      </c>
+      <c r="H6" s="8" t="n">
+        <v>7652</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5" t="n">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="n">
         <v>174000</v>
       </c>
       <c r="C7" s="1" t="n">
@@ -464,12 +579,24 @@
       <c r="D7" s="1" t="n">
         <v>32000</v>
       </c>
+      <c r="E7" s="7" t="n">
+        <v>52.7487924035376</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>331.1</v>
+      </c>
+      <c r="H7" s="8" t="n">
+        <v>2200</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="5" t="n">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="n">
         <v>101000</v>
       </c>
       <c r="C8" s="1" t="n">
@@ -478,12 +605,24 @@
       <c r="D8" s="1" t="n">
         <v>37300</v>
       </c>
+      <c r="E8" s="7" t="n">
+        <v>103.135497865392</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>262.23</v>
+      </c>
+      <c r="H8" s="8" t="n">
+        <v>12035</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5" t="n">
+      <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="n">
         <v>183000</v>
       </c>
       <c r="C9" s="1" t="n">
@@ -492,12 +631,24 @@
       <c r="D9" s="1" t="n">
         <v>27500</v>
       </c>
+      <c r="E9" s="7" t="n">
+        <v>67.4253996819285</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>385.35</v>
+      </c>
+      <c r="H9" s="8" t="n">
+        <v>4455</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="5" t="n">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6" t="n">
         <v>170000</v>
       </c>
       <c r="C10" s="1" t="n">
@@ -506,12 +657,24 @@
       <c r="D10" s="1" t="n">
         <v>26700</v>
       </c>
+      <c r="E10" s="7" t="n">
+        <v>69.0101283231739</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>341.98</v>
+      </c>
+      <c r="H10" s="8" t="n">
+        <v>6157</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="5" t="n">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6" t="n">
         <v>144000</v>
       </c>
       <c r="C11" s="1" t="n">
@@ -520,12 +683,24 @@
       <c r="D11" s="1" t="n">
         <v>26300</v>
       </c>
+      <c r="E11" s="7" t="n">
+        <v>58.5434300457158</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>333.87</v>
+      </c>
+      <c r="H11" s="8" t="n">
+        <v>4130</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="5" t="n">
+      <c r="A12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="6" t="n">
         <v>124000</v>
       </c>
       <c r="C12" s="1" t="n">
@@ -534,12 +709,24 @@
       <c r="D12" s="1" t="n">
         <v>27600</v>
       </c>
+      <c r="E12" s="7" t="n">
+        <v>71.570526797395</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>286.19</v>
+      </c>
+      <c r="H12" s="8" t="n">
+        <v>6046</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="5" t="n">
+      <c r="A13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="6" t="n">
         <v>112000</v>
       </c>
       <c r="C13" s="1" t="n">
@@ -548,12 +735,24 @@
       <c r="D13" s="1" t="n">
         <v>29400</v>
       </c>
+      <c r="E13" s="7" t="n">
+        <v>91.1540402009316</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>279.67</v>
+      </c>
+      <c r="H13" s="8" t="n">
+        <v>14681</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="5" t="n">
+      <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="n">
         <v>94000</v>
       </c>
       <c r="C14" s="1" t="n">
@@ -562,12 +761,24 @@
       <c r="D14" s="1" t="n">
         <v>33200</v>
       </c>
+      <c r="E14" s="7" t="n">
+        <v>98.1275117726296</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>185.43</v>
+      </c>
+      <c r="H14" s="8" t="n">
+        <v>11308</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="5" t="n">
+      <c r="A15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="n">
         <v>138000</v>
       </c>
       <c r="C15" s="1" t="n">
@@ -576,12 +787,24 @@
       <c r="D15" s="1" t="n">
         <v>27100</v>
       </c>
+      <c r="E15" s="7" t="n">
+        <v>85.8104298422344</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>270.62</v>
+      </c>
+      <c r="H15" s="8" t="n">
+        <v>9143</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="5" t="n">
+      <c r="A16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="6" t="n">
         <v>129000</v>
       </c>
       <c r="C16" s="1" t="n">
@@ -590,12 +813,24 @@
       <c r="D16" s="1" t="n">
         <v>27600</v>
       </c>
+      <c r="E16" s="7" t="n">
+        <v>45.4629510516498</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>250.15</v>
+      </c>
+      <c r="H16" s="8" t="n">
+        <v>4957</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="5" t="n">
+      <c r="A17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6" t="n">
         <v>130000</v>
       </c>
       <c r="C17" s="1" t="n">
@@ -604,12 +839,24 @@
       <c r="D17" s="1" t="n">
         <v>27900</v>
       </c>
+      <c r="E17" s="7" t="n">
+        <v>58.0735255139784</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>257.81</v>
+      </c>
+      <c r="H17" s="8" t="n">
+        <v>2300</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="5" t="n">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="n">
         <v>142000</v>
       </c>
       <c r="C18" s="1" t="n">
@@ -618,12 +865,24 @@
       <c r="D18" s="1" t="n">
         <v>27100</v>
       </c>
+      <c r="E18" s="7" t="n">
+        <v>63.4606292834685</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>304.82</v>
+      </c>
+      <c r="H18" s="8" t="n">
+        <v>2700</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="5" t="n">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="6" t="n">
         <v>135000</v>
       </c>
       <c r="C19" s="1" t="n">
@@ -632,12 +891,24 @@
       <c r="D19" s="1" t="n">
         <v>26400</v>
       </c>
+      <c r="E19" s="7" t="n">
+        <v>71.3250399241717</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>270.78</v>
+      </c>
+      <c r="H19" s="8" t="n">
+        <v>4837</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="5" t="n">
+      <c r="A20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="6" t="n">
         <v>106000</v>
       </c>
       <c r="C20" s="1" t="n">
@@ -646,12 +917,24 @@
       <c r="D20" s="1" t="n">
         <v>33400</v>
       </c>
+      <c r="E20" s="7" t="n">
+        <v>99.8604341571297</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>239.14</v>
+      </c>
+      <c r="H20" s="8" t="n">
+        <v>16097</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="5" t="n">
+      <c r="A21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="6" t="n">
         <v>68000</v>
       </c>
       <c r="C21" s="1" t="n">
@@ -660,12 +943,24 @@
       <c r="D21" s="1" t="n">
         <v>40400</v>
       </c>
+      <c r="E21" s="7" t="n">
+        <v>109.783954162041</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>156.2</v>
+      </c>
+      <c r="H21" s="8" t="n">
+        <v>12884</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="5" t="n">
+      <c r="A22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="6" t="n">
         <v>79000</v>
       </c>
       <c r="C22" s="1" t="n">
@@ -674,12 +969,24 @@
       <c r="D22" s="1" t="n">
         <v>32400</v>
       </c>
+      <c r="E22" s="7" t="n">
+        <v>49.6232404163378</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>175.47</v>
+      </c>
+      <c r="H22" s="8" t="n">
+        <v>4709</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="5" t="n">
+      <c r="A23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="6" t="n">
         <v>162000</v>
       </c>
       <c r="C23" s="1" t="n">
@@ -688,12 +995,24 @@
       <c r="D23" s="1" t="n">
         <v>29900</v>
       </c>
+      <c r="E23" s="7" t="n">
+        <v>90.8389497118112</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>325.92</v>
+      </c>
+      <c r="H23" s="8" t="n">
+        <v>12157</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="5" t="n">
+      <c r="A24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="6" t="n">
         <v>140000</v>
       </c>
       <c r="C24" s="1" t="n">
@@ -702,12 +1021,24 @@
       <c r="D24" s="1" t="n">
         <v>27300</v>
       </c>
+      <c r="E24" s="7" t="n">
+        <v>68.420860842689</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>303.54</v>
+      </c>
+      <c r="H24" s="8" t="n">
+        <v>8636</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="5" t="n">
+      <c r="A25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="6" t="n">
         <v>111000</v>
       </c>
       <c r="C25" s="1" t="n">
@@ -716,12 +1047,24 @@
       <c r="D25" s="1" t="n">
         <v>30200</v>
       </c>
+      <c r="E25" s="7" t="n">
+        <v>53.5192582512718</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>206.19</v>
+      </c>
+      <c r="H25" s="8" t="n">
+        <v>5480</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="5" t="n">
+      <c r="A26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="6" t="n">
         <v>141000</v>
       </c>
       <c r="C26" s="1" t="n">
@@ -730,12 +1073,24 @@
       <c r="D26" s="1" t="n">
         <v>24100</v>
       </c>
+      <c r="E26" s="7" t="n">
+        <v>77.1486723483627</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>352.01</v>
+      </c>
+      <c r="H26" s="8" t="n">
+        <v>9723</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="5" t="n">
+      <c r="A27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="6" t="n">
         <v>136000</v>
       </c>
       <c r="C27" s="1" t="n">
@@ -744,12 +1099,24 @@
       <c r="D27" s="1" t="n">
         <v>28000</v>
       </c>
+      <c r="E27" s="7" t="n">
+        <v>56.6852353725493</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>303.86</v>
+      </c>
+      <c r="H27" s="8" t="n">
+        <v>5386</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="5" t="n">
+      <c r="A28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="6" t="n">
         <v>108000</v>
       </c>
       <c r="C28" s="1" t="n">
@@ -758,12 +1125,24 @@
       <c r="D28" s="1" t="n">
         <v>36100</v>
       </c>
+      <c r="E28" s="7" t="n">
+        <v>49.9371955516069</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>196.9</v>
+      </c>
+      <c r="H28" s="8" t="n">
+        <v>3400</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="5" t="n">
+      <c r="A29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="6" t="n">
         <v>146000</v>
       </c>
       <c r="C29" s="1" t="n">
@@ -772,12 +1151,24 @@
       <c r="D29" s="1" t="n">
         <v>29400</v>
       </c>
+      <c r="E29" s="7" t="n">
+        <v>87.8894589477784</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>317.26</v>
+      </c>
+      <c r="H29" s="8" t="n">
+        <v>10992</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="5" t="n">
+      <c r="A30" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="6" t="n">
         <v>103000</v>
       </c>
       <c r="C30" s="1" t="n">
@@ -786,12 +1177,24 @@
       <c r="D30" s="1" t="n">
         <v>28200</v>
       </c>
+      <c r="E30" s="7" t="n">
+        <v>45.0103847295025</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>204.53</v>
+      </c>
+      <c r="H30" s="8" t="n">
+        <v>4665</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="5" t="n">
+      <c r="A31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="6" t="n">
         <v>136000</v>
       </c>
       <c r="C31" s="1" t="n">
@@ -800,12 +1203,24 @@
       <c r="D31" s="1" t="n">
         <v>30200</v>
       </c>
+      <c r="E31" s="7" t="n">
+        <v>85.3031287107927</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>317.71</v>
+      </c>
+      <c r="H31" s="8" t="n">
+        <v>16057</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="5" t="n">
+      <c r="A32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="6" t="n">
         <v>138000</v>
       </c>
       <c r="C32" s="1" t="n">
@@ -814,12 +1229,24 @@
       <c r="D32" s="1" t="n">
         <v>25500</v>
       </c>
+      <c r="E32" s="7" t="n">
+        <v>64.8883604079132</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>276.7</v>
+      </c>
+      <c r="H32" s="8" t="n">
+        <v>7130</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="5" t="n">
+      <c r="A33" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="6" t="n">
         <v>171000</v>
       </c>
       <c r="C33" s="1" t="n">
@@ -828,12 +1255,24 @@
       <c r="D33" s="1" t="n">
         <v>34500</v>
       </c>
+      <c r="E33" s="7" t="n">
+        <v>65.8312664506985</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>329.67</v>
+      </c>
+      <c r="H33" s="8" t="n">
+        <v>9528</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="5" t="n">
+      <c r="A34" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="6" t="n">
         <v>98000</v>
       </c>
       <c r="C34" s="1" t="n">
@@ -841,6 +1280,18 @@
       </c>
       <c r="D34" s="1" t="n">
         <v>39700</v>
+      </c>
+      <c r="E34" s="7" t="n">
+        <v>171.290799389372</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>255.32</v>
+      </c>
+      <c r="H34" s="8" t="n">
+        <v>11883</v>
       </c>
     </row>
   </sheetData>

</xml_diff>